<commit_message>
Updated Agent Portal with Protected Routes
</commit_message>
<xml_diff>
--- a/frontend/List.xlsx
+++ b/frontend/List.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>firstName</t>
   </si>
@@ -41,6 +41,12 @@
   </si>
   <si>
     <t>ething</t>
+  </si>
+  <si>
+    <t>Soumyadip</t>
+  </si>
+  <si>
+    <t>hjhjkj</t>
   </si>
   <si>
     <t>Jane</t>
@@ -64,13 +70,13 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -424,7 +430,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
@@ -435,7 +441,7 @@
     <col min="3" max="3" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -450,7 +456,7 @@
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="2">
         <v>1234567890</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -461,7 +467,7 @@
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="3">
         <v>45665456</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -472,22 +478,33 @@
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="3">
         <v>65645</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="3">
-        <v>9876543210</v>
+      <c r="B5" s="4">
+        <v>65222</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
+      <c r="A6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="2">
+        <v>9876543210</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>